<commit_message>
TVöD VKA mit Beschreibung in letzter Zeile
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="tvaoed-pfege" sheetId="1" state="visible" r:id="rId2"/>
@@ -311,6 +311,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -370,16 +371,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,49 +408,49 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="79.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="79.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1190.69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>1252.07</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>1353.38</v>
       </c>
     </row>
@@ -468,424 +473,424 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>4129.77</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>4255.33</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4804.44</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>5216.23</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>5833.95</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>6211.42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3751.26</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>4083.75</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>4529.86</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>4804.44</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>5353.48</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>5676.08</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>3662.48</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>3994.55</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>4296.52</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>4667.14</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>5078.96</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>5326.04</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>3525.89</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>3843.52</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>4118.1</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>4433.81</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>4941.69</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>5161.3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>3507.36</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>3804.1</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>4109.21</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>4419.58</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>4762.78</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>5002.98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>3447.95</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>3708.47</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>4049.44</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>4323.95</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>4667.14</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>4838.72</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>3400.6</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>3697.96</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>4024.89</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>4313.15</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>4670.07</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>4821.07</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>3312.44</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>3645.37</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>3819.73</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>4258.98</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>4602.18</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>4808.08</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>3244.38</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>3575.21</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>3748.45</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>4186.72</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>4529.86</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>4735.78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>3096.29</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>3416.24</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>3576.22</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>4050.58</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>4435.04</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>4750.84</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>3012.84</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>3299.02</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>3561.97</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>3944.47</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>4303.05</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>4577.98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>3012.84</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>3299.02</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>3561.97</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>3944.47</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>4303.05</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>4577.98</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>2969.94</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>3227.29</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>3454.4</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>3669.56</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>3878.72</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>4096.87</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>2898.63</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>3142.08</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>3355.33</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>3568.53</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>3728.47</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>3967.08</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>2744.34</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>3002.13</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>3188.73</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>3315.33</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>3435.29</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>3622.14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>2567.24</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>2824.89</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>3004.13</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>3168.73</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>3244.03</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>3333.99</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>2468.79</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>2681.96</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>2743.16</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>2841.06</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>2920.62</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>2987.93</v>
       </c>
     </row>
@@ -908,401 +913,401 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D4 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="1:1 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>5017.31</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>5394.35</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>5593.59</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>6301.27</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>6837.15</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>7042.26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>4542.64</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>4885.93</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5167.63</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>5593.59</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>6246.27</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>6433.67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>4188.38</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>4508.07</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>4748.54</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>5215.72</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>5861.53</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>6037.38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>3774.86</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>4040.88</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>4604.26</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>5098.93</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>5737.87</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>5910</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>3652.64</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>3898.38</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>4178.29</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>4604.26</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>5222.6</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>5379.28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>3523.62</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>3764.77</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>4040.88</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>4322.55</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>4858.48</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>5004.24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>3136.59</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>3369.08</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>3520.54</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>3939.07</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>4295.09</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>4423.96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>3136.59</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>3369.08</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>3419.58</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>3520.54</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>3939.07</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>4055.96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>2946.46</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>3173.48</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>3299.66</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>3419.58</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>3552.1</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>3634.13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>2772.35</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>2994.05</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>3160.84</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>3287.05</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>3388.03</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>3476.36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>2725.66</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>2945.1</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>3067.49</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>3192.41</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>3274.43</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>3362.77</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>2618.93</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>2834.95</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>2957.34</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>3073.61</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>3167.15</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>3230.26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>2500.7</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>2718.69</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>2871.67</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>2957.34</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>3043.02</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>3098.08</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>2468.79</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>2681.96</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>2743.16</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>2841.06</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>2920.62</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>2987.93</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>2302.84</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>2504.49</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>2565.69</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>2626.88</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>2767.62</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>2914.51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>2094.49</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>2125.06</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>2161.78</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>2198.51</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>2290.3</v>
       </c>
     </row>
@@ -1324,83 +1329,83 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="1:1 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>6122.63</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>6795.9</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>7434.88</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>7853.95</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>7957.04</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>4508.07</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>4748.54</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>5167.63</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>5593.59</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>6246.27</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>6433.67</v>
       </c>
     </row>
@@ -1423,53 +1428,53 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1876.21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1876.21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>1876.21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>1652.02</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>1595.36</v>
       </c>
     </row>
@@ -1492,53 +1497,53 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="D4 C6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="1:1 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1903.54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>1903.54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>1903.54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>1678.26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>1621.31</v>
       </c>
     </row>
@@ -1561,424 +1566,424 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D4 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="1:1 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>4025.78</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>4133.45</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4666.83</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>5066.83</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>5666.85</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>6033.52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3696.23</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>3966.79</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>4400.13</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>4666.83</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>5200.16</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>5513.51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>3616.47</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>3880.13</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>4173.46</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>4533.47</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>4933.48</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>5173.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>3481.65</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>3733.42</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>4000.14</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>4306.81</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>4800.16</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>5013.48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>3446.47</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>3695.15</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>3991.52</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>4292.99</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>4626.36</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>4859.69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>3361.11</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>3603.41</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>3933.46</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>4200.11</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>4533.47</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>4700.14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>3351.74</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>3593.37</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>3909.61</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>4189.61</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>4536.3</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>4682.97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>3304.79</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>3542.98</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>3710.32</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>4137.01</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>4470.35</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>4670.36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>3242.17</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>3475.77</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>3641.71</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>4066.8</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>4400.13</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>4600.14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>3017.83</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>3324.4</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>3477.7</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>3935.68</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>4309.24</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>4616.08</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>2995.63</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>3211.18</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>3463.08</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>3831.49</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>4179.82</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>4446.86</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>2995.63</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>3211.18</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>3463.08</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>3831.49</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>4179.82</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>4446.86</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>2931.61</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>3142.47</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>3360.03</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>3566.15</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>3767.64</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>3979.52</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>2855.54</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>3060.84</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>3265.12</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>3469.36</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>3622.58</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>3853.46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>2730.63</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>2926.79</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>3105.53</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>3226.82</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>3341.72</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>3520.72</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>2572.41</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>2756.99</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>2928.7</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>3086.37</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>3158.51</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>3244.68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>2377.38</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>2490.44</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>2574.07</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>2664.88</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>2767</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>2869.15</v>
       </c>
     </row>
@@ -2001,421 +2006,421 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D4 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="1:1 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>5017.06</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>5358.22</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>5738.77</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>6258.28</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>6792.69</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>7144.27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>4542.98</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>4851.9</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5255.33</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>5703.01</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>6202.05</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>6560.31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>4187.45</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>4526.02</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>4911.44</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>5329.9</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>5822.3</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>6089.52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>3752.91</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>4142.5</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>4597.79</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>5102.97</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>5695.74</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>5977</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>3622.16</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>3980.48</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>4317.18</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>4682.47</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>5182.41</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>5463.69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>3492.26</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>3773.01</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>4092.18</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>4438.33</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>4823.79</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>4950.36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>3361.34</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>3604.55</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>3908.13</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>4238.9</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>4597.52</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>4712.64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>3230.42</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>3341.54</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>3619.82</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>3925.18</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>4261.26</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>4542.51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>3099.5</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>3306.81</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>3363.83</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>3556.55</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>3909.66</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>4049.38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>2910.37</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>3104.82</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>3239.51</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>3373.97</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>3518.19</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>3587.54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>2733.87</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>2957.9</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>3091.36</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>3226.04</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>3353.07</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>3421.28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>2683.45</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>2867.82</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>2997.1</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>3125.04</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>3250.7</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>3314.71</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>2576.29</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>2755.14</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>2875.93</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>3003.85</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>3122.72</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>3184.15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>2456.51</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>2637.49</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>2789.34</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>2883.87</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>2978.39</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>3033.74</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>2418.66</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>2613.29</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>2660.65</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>2768.92</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>2850.16</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>2924.58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>2242.16</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>2439.13</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>2486.89</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>2555.05</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>2704.86</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>2861.58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>2015.52</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>2048.86</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>2090.55</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>2129.42</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>2229.47</v>
       </c>
     </row>
@@ -2437,426 +2442,435 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D4 B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>5017.06</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>5358.22</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>5738.77</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>6258.28</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>6792.69</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>7144.27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>4542.98</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>4851.9</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>5255.33</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>5703.01</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>6202.05</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>6560.31</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>4187.45</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>4526.02</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>4911.44</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>5329.9</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>5822.3</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>6089.52</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>3752.91</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>4142.5</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>4597.79</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>5102.97</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>5695.74</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>5977</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>3622.16</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>3980.48</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>4317.18</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>4682.47</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>5182.41</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>5463.69</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>3492.26</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>3773.01</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>4092.18</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>4438.33</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>4823.79</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>4950.36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>3390.37</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>3640.83</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>3913.2</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>4206.69</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>4522.19</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>4748.36</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>3180.94</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>3415.7</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>3563</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>3998.95</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>4257.27</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>4556.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>3069.16</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>3271.39</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>3468.21</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>3906.05</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>4005.11</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>4258.04</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>2910.37</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>3104.82</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>3239.51</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>3373.97</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>3518.19</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>3587.54</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>2733.87</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>2957.9</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>3091.36</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>3226.04</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>3353.07</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>3421.28</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>2683.45</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>2867.82</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>2997.1</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>3125.04</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>3250.7</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>3314.71</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>2576.29</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>2755.14</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>2875.93</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>3003.85</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>3122.72</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>3184.15</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>2456.51</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>2637.49</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>2789.34</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>2883.87</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>2978.39</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>3033.74</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>2418.66</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>2613.29</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>2660.65</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>2768.92</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>2850.16</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>2924.58</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>2242.16</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>2439.13</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>2486.89</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>2555.05</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>2704.86</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>2861.58</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>2015.52</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>2048.86</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>2090.55</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>2129.42</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>2229.47</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>5017.06</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>5358.22</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>5738.77</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>6258.28</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>6792.69</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>7144.27</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>4542.98</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>4851.9</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>5255.33</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>5703.01</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>6202.05</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>6560.31</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>4187.45</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>4526.02</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>4911.44</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>5329.9</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>5822.3</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>6089.52</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>3752.91</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>4142.5</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>4597.79</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>5102.97</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>5695.74</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>5977</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>3622.16</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>3980.48</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>4317.18</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>4682.47</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>5182.41</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>5463.69</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>3492.26</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>3773.01</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>4092.18</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>4438.33</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>4823.79</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>4950.36</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>3390.37</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>3640.83</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>3913.2</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>4206.69</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>4522.19</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>4748.36</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>3180.94</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>3415.7</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>3563</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>3998.95</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>4257.27</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>4556.5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>3069.16</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>3271.39</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>3468.21</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>3906.05</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>4005.11</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>4258.04</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>2910.37</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>3104.82</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>3239.51</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>3373.97</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>3518.19</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>3587.54</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>2733.87</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>2957.9</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>3091.36</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>3226.04</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>3353.07</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>3421.28</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>2683.45</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>2867.82</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>2997.1</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>3125.04</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>3250.7</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>3314.71</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>2576.29</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>2755.14</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>2875.93</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>3003.85</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>3122.72</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>3184.15</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>2456.51</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>2637.49</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>2789.34</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>2883.87</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>2978.39</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>3033.74</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>2418.66</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>2613.29</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>2660.65</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>2768.92</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>2850.16</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>2924.58</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>2242.16</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>2439.13</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>2486.89</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>2555.05</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>2704.86</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>2861.58</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>2015.52</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>2048.86</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>2090.55</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>2129.42</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>2229.47</v>
-      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A19:G19"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2875,85 +2889,85 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>87.43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>87.43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>88.14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>88.14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>74.35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>74.35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>46.47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>46.47</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>32.53</v>
       </c>
     </row>
@@ -2976,37 +2990,37 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="D4 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="1:1 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>60</v>
       </c>
     </row>
@@ -3029,53 +3043,53 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="D4 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="1:1 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>84.51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>84.51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>70.28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>70.28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>51.78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Titel raus – nur noch Zahlenwerte
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="sue-vka" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
   <si>
     <t xml:space="preserve">Stufe 1</t>
   </si>
@@ -102,10 +102,6 @@
     <t xml:space="preserve"> S 2 </t>
   </si>
   <si>
-    <t xml:space="preserve">Sozial- und Erziehungsdienst VKA ab 1. April 2022 (Monatsentgelt in Euro)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve"> EG 15 </t>
   </si>
   <si>
@@ -157,13 +153,6 @@
     <t xml:space="preserve"> EG 1 </t>
   </si>
   <si>
-    <t xml:space="preserve">TVöD-VKA ab 1. April 2022 (Monatsentgelt in Euro)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TVöD-Bund ab 1. April 2022 (Monatsentgelt in Euro)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> EG 1-8 </t>
   </si>
   <si>
@@ -173,20 +162,12 @@
     <t xml:space="preserve"> EG 13-15</t>
   </si>
   <si>
-    <t xml:space="preserve">Jahressonderzahlung TvöD-Bund (in Prozent eines Monatsgehalts)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">S 2 - S 9</t>
   </si>
   <si>
     <t xml:space="preserve">S 10 - S 18</t>
   </si>
   <si>
-    <t xml:space="preserve">Jahressonderzahlung TvöD-VKA (in Prozent eines Monatsgehalts)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Praktikum als Sozialarbeiter*in</t>
   </si>
   <si>
@@ -196,30 +177,18 @@
     <t xml:space="preserve">Praktikum als Heilpädagog*in</t>
   </si>
   <si>
-    <t xml:space="preserve">Praktikum als </t>
+    <t xml:space="preserve">Praktikum als Erzieher*in</t>
   </si>
   <si>
     <t xml:space="preserve">Praktikum als Kinderpfleger*in</t>
   </si>
   <si>
-    <t xml:space="preserve">TVPöD ab 1. April 2022 (in Euro)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ab 1. April 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> in Euro</t>
-  </si>
-  <si>
     <t xml:space="preserve">im ersten Ausbildungsjahr</t>
   </si>
   <si>
     <t xml:space="preserve">im zweiten Ausbildungsjahr</t>
   </si>
   <si>
-    <t xml:space="preserve">TVAöD Pflege – Ausbildungsentgelte für Erzieher*innen in der praxisintegrierten Ausbildung (PiA) </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Stufe 1 </t>
   </si>
   <si>
@@ -238,18 +207,6 @@
     <t xml:space="preserve"> Stufe 6 </t>
   </si>
   <si>
-    <t xml:space="preserve">TV-L –  ab 1. Dezember 2022 (Monatsentgelt in Euro) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TV-L: Sozial- und Erziehungsdienst  – ab 1. Dezember 2022 (Monatsentgelt in Euro)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Praktikum als Erzieher*in</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TV Prakt-L ab 1. Dezember 2022 (in Euro)</t>
-  </si>
-  <si>
     <t xml:space="preserve">EG 1-4 </t>
   </si>
   <si>
@@ -277,10 +234,6 @@
     <t xml:space="preserve"> EG 14-15 </t>
   </si>
   <si>
-    <t xml:space="preserve">Jahressonderzahlung TV-L (in Prozent eines Monatsgehalts)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stufe 4a</t>
   </si>
   <si>
@@ -291,9 +244,6 @@
   </si>
   <si>
     <t xml:space="preserve">13Ü</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TV-L Überleitungsgruppen ab 1. Dezember 2022</t>
   </si>
 </sst>
 </file>
@@ -400,8 +350,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -817,10 +767,8 @@
         <v>2869.15</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>23</v>
-      </c>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -841,14 +789,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="n">
         <v>1903.54</v>
@@ -856,7 +804,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1903.54</v>
@@ -864,7 +812,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1903.54</v>
@@ -872,7 +820,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1678.26</v>
@@ -880,16 +828,14 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1621.31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -910,14 +856,14 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>87.43</v>
@@ -925,7 +871,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>87.43</v>
@@ -933,7 +879,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>88.14</v>
@@ -941,7 +887,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>88.14</v>
@@ -949,7 +895,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>74.35</v>
@@ -957,7 +903,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>74.35</v>
@@ -965,7 +911,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>46.47</v>
@@ -973,7 +919,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>46.47</v>
@@ -981,16 +927,14 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>32.53</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>80</v>
-      </c>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1011,7 +955,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1030,10 +974,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1044,7 +988,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>6122.63</v>
@@ -1064,7 +1008,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>4508.07</v>
@@ -1086,9 +1030,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1109,7 +1051,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1136,7 +1078,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>5017.06</v>
@@ -1159,7 +1101,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>4542.98</v>
@@ -1182,7 +1124,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>4187.45</v>
@@ -1205,7 +1147,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3752.91</v>
@@ -1228,7 +1170,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>3622.16</v>
@@ -1251,7 +1193,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>3492.26</v>
@@ -1274,7 +1216,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>3390.37</v>
@@ -1297,7 +1239,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>3180.94</v>
@@ -1320,7 +1262,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>3069.16</v>
@@ -1343,7 +1285,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>2910.37</v>
@@ -1366,7 +1308,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>2733.87</v>
@@ -1389,7 +1331,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>2683.45</v>
@@ -1412,7 +1354,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>2576.29</v>
@@ -1435,7 +1377,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>2456.51</v>
@@ -1458,7 +1400,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>2418.66</v>
@@ -1481,7 +1423,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>2242.16</v>
@@ -1504,7 +1446,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>2015.52</v>
@@ -1523,9 +1465,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1555,7 +1495,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1582,7 +1522,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>5017.06</v>
@@ -1605,7 +1545,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>4542.98</v>
@@ -1628,7 +1568,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>4187.45</v>
@@ -1651,7 +1591,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3752.91</v>
@@ -1674,7 +1614,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>3622.16</v>
@@ -1697,7 +1637,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>3492.26</v>
@@ -1720,7 +1660,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>3361.34</v>
@@ -1743,7 +1683,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>3230.42</v>
@@ -1766,7 +1706,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>3099.5</v>
@@ -1789,7 +1729,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>2910.37</v>
@@ -1812,7 +1752,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>2733.87</v>
@@ -1835,7 +1775,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>2683.45</v>
@@ -1858,7 +1798,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>2576.29</v>
@@ -1881,7 +1821,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>2456.51</v>
@@ -1904,7 +1844,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>2418.66</v>
@@ -1927,7 +1867,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>2242.16</v>
@@ -1950,7 +1890,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>2015.52</v>
@@ -1969,9 +1909,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1991,7 +1929,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1999,7 +1937,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>90</v>
@@ -2007,7 +1945,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>80</v>
@@ -2015,16 +1953,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2045,14 +1981,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>84.51</v>
@@ -2060,7 +1996,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>84.51</v>
@@ -2068,7 +2004,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>70.28</v>
@@ -2076,7 +2012,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>70.28</v>
@@ -2084,16 +2020,14 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>51.78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="A6" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2114,14 +2048,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>1876.21</v>
@@ -2129,7 +2063,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1876.21</v>
@@ -2137,7 +2071,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1876.21</v>
@@ -2145,7 +2079,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>1652.02</v>
@@ -2153,16 +2087,14 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>1595.36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2180,10 +2112,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2194,39 +2126,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1190.69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1190.69</v>
+        <v>1252.07</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>1252.07</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="1" t="n">
         <v>1353.38</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2248,34 +2167,34 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>5017.31</v>
@@ -2298,7 +2217,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>4542.64</v>
@@ -2321,7 +2240,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>4188.38</v>
@@ -2344,7 +2263,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3774.86</v>
@@ -2367,7 +2286,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>3652.64</v>
@@ -2390,7 +2309,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>3523.62</v>
@@ -2413,7 +2332,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>3136.59</v>
@@ -2436,7 +2355,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>3136.59</v>
@@ -2459,7 +2378,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>2946.46</v>
@@ -2482,7 +2401,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>2772.35</v>
@@ -2505,7 +2424,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>2725.66</v>
@@ -2528,7 +2447,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>2618.93</v>
@@ -2551,7 +2470,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>2500.7</v>
@@ -2574,7 +2493,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>2468.79</v>
@@ -2597,7 +2516,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>2302.84</v>
@@ -2620,7 +2539,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="n">
@@ -2640,9 +2559,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="A18" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2663,29 +2580,29 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3080,9 +2997,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>